<commit_message>
HWV 0.3.0: Core64c Logic Board, add and rename data sheets, update BOM notes for JLCPCB component availability
</commit_message>
<xml_diff>
--- a/Electronics/Core64c LB V0.3/Core64c LB V0.3 2022-05-17 Gerbers/Core64c LB v0.3 2021-05-17 BOM.xlsx
+++ b/Electronics/Core64c LB V0.3/Core64c LB V0.3 2022-05-17 Gerbers/Core64c LB v0.3 2021-05-17 BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ageppert/Dropbox/Electronics/Core 64 Interactive Badge/Core-64c-Compact-Interactive-Core-Memory-Badge/Electronics/Core64c LB V0.3/Core64c LB V0.3 2022-05-17 Gerbers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7823553-F7C2-1F47-A004-D5B19FFEEF0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84BD2EBE-628B-C140-93E3-695C21FEA65B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19700" yWindow="7260" windowWidth="27240" windowHeight="20740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19680" yWindow="7160" windowWidth="27240" windowHeight="20740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Core64C LB v0.3 BOM" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="200">
   <si>
     <t>Footprint</t>
   </si>
@@ -1282,8 +1282,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>393700</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1219200</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
@@ -1343,8 +1343,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>393700</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1219200</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
@@ -1404,8 +1404,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>393700</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1219200</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
@@ -1465,8 +1465,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>393700</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1219200</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
@@ -1526,8 +1526,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>393700</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1219200</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
@@ -1587,8 +1587,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>393700</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1219200</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
@@ -1648,8 +1648,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>393700</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1219200</xdr:colOff>
       <xdr:row>27</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
@@ -1709,8 +1709,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>393700</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1219200</xdr:colOff>
       <xdr:row>30</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
@@ -1770,8 +1770,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>393700</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1219200</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
@@ -1831,8 +1831,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>393700</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1219200</xdr:colOff>
       <xdr:row>36</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
@@ -1892,8 +1892,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>393700</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1219200</xdr:colOff>
       <xdr:row>39</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
@@ -1953,8 +1953,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>393700</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1219200</xdr:colOff>
       <xdr:row>42</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
@@ -2014,8 +2014,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>393700</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1219200</xdr:colOff>
       <xdr:row>45</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
@@ -2075,8 +2075,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>393700</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1219200</xdr:colOff>
       <xdr:row>48</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
@@ -2136,8 +2136,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>393700</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1219200</xdr:colOff>
       <xdr:row>51</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
@@ -2197,8 +2197,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>393700</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1219200</xdr:colOff>
       <xdr:row>54</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
@@ -2258,8 +2258,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>393700</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1219200</xdr:colOff>
       <xdr:row>57</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
@@ -2319,8 +2319,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>393700</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1219200</xdr:colOff>
       <xdr:row>60</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
@@ -2380,8 +2380,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>393700</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1219200</xdr:colOff>
       <xdr:row>63</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
@@ -2441,8 +2441,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>393700</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1219200</xdr:colOff>
       <xdr:row>66</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
@@ -2502,8 +2502,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>393700</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1219200</xdr:colOff>
       <xdr:row>69</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
@@ -2563,8 +2563,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>393700</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1219200</xdr:colOff>
       <xdr:row>72</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
@@ -2624,8 +2624,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>393700</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1219200</xdr:colOff>
       <xdr:row>75</xdr:row>
       <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
@@ -2685,8 +2685,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>393700</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1219200</xdr:colOff>
       <xdr:row>78</xdr:row>
       <xdr:rowOff>50800</xdr:rowOff>
     </xdr:to>
@@ -2738,6 +2738,49 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="304800" cy="304800"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="27" name="AutoShape 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7920F77B-F19A-B144-9C66-A4363BF570A5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="482600"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3041,7 +3084,7 @@
   <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="A24" sqref="A24:D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3390,6 +3433,9 @@
       <c r="D24" t="s">
         <v>73</v>
       </c>
+      <c r="E24" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
@@ -3457,940 +3503,922 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{489B376F-CCE8-D948-97BA-EB41C11191C0}">
-  <dimension ref="A1:E77"/>
+  <dimension ref="A1:F77"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E77"/>
+      <selection activeCell="B12" sqref="B12:B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="26.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
-    </row>
-    <row r="4" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="B3" s="2"/>
+    </row>
+    <row r="4" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="A4" s="3"/>
+      <c r="B4" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C4" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="7" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="7"/>
+      <c r="C5" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="C5" s="7">
+      <c r="D5" s="7">
         <v>30</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="E5" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="F5" s="7" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+    <row r="6" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="B6" s="7"/>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
-    </row>
-    <row r="7" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="F6" s="7"/>
+    </row>
+    <row r="7" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="B7" s="7"/>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
-    </row>
-    <row r="8" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="F7" s="7"/>
+    </row>
+    <row r="8" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="7"/>
+      <c r="C8" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="C8" s="7">
+      <c r="D8" s="7">
         <v>110</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="E8" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="F8" s="7" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+    <row r="9" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="B9" s="7"/>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>
-    </row>
-    <row r="10" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+      <c r="F9" s="7"/>
+    </row>
+    <row r="10" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="A10" s="5"/>
+      <c r="B10" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="B10" s="7"/>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
       <c r="E10" s="7"/>
-    </row>
-    <row r="11" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="F10" s="7"/>
+    </row>
+    <row r="11" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="7"/>
+      <c r="C11" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="C11" s="7">
+      <c r="D11" s="7">
         <v>10</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="E11" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="F11" s="7" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+    <row r="12" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="A12" s="4"/>
+      <c r="B12" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="B12" s="7"/>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
       <c r="E12" s="7"/>
-    </row>
-    <row r="13" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+      <c r="F12" s="7"/>
+    </row>
+    <row r="13" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="A13" s="5"/>
+      <c r="B13" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="B13" s="7"/>
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
-    </row>
-    <row r="14" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="F13" s="7"/>
+    </row>
+    <row r="14" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="7"/>
+      <c r="C14" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="C14" s="7">
+      <c r="D14" s="7">
         <v>54</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="E14" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="E14" s="7" t="s">
+      <c r="F14" s="7" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+    <row r="15" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="B15" s="7"/>
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
-    </row>
-    <row r="16" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
+      <c r="F15" s="7"/>
+    </row>
+    <row r="16" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="A16" s="5"/>
+      <c r="B16" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="B16" s="7"/>
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
       <c r="E16" s="7"/>
-    </row>
-    <row r="17" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="F16" s="7"/>
+    </row>
+    <row r="17" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="7"/>
+      <c r="C17" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="C17" s="7">
+      <c r="D17" s="7">
         <v>5</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="E17" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="E17" s="7" t="s">
+      <c r="F17" s="7" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
+    <row r="18" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="B18" s="7"/>
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
       <c r="E18" s="7"/>
-    </row>
-    <row r="19" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
+      <c r="F18" s="7"/>
+    </row>
+    <row r="19" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="A19" s="5"/>
+      <c r="B19" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="B19" s="7"/>
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
       <c r="E19" s="7"/>
-    </row>
-    <row r="20" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="F19" s="7"/>
+    </row>
+    <row r="20" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="7"/>
+      <c r="C20" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="C20" s="7">
+      <c r="D20" s="7">
         <v>15</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="E20" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="E20" s="7" t="s">
+      <c r="F20" s="7" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
+    <row r="21" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="A21" s="4"/>
+      <c r="B21" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="B21" s="7"/>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
       <c r="E21" s="7"/>
-    </row>
-    <row r="22" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
+      <c r="F21" s="7"/>
+    </row>
+    <row r="22" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="A22" s="5"/>
+      <c r="B22" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="B22" s="7"/>
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
       <c r="E22" s="7"/>
-    </row>
-    <row r="23" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="F22" s="7"/>
+    </row>
+    <row r="23" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
-      <c r="B23" s="7" t="s">
+      <c r="B23" s="7"/>
+      <c r="C23" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="C23" s="7">
+      <c r="D23" s="7">
         <v>34</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="E23" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="E23" s="7" t="s">
+      <c r="F23" s="7" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
+    <row r="24" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="A24" s="4"/>
+      <c r="B24" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="B24" s="7"/>
       <c r="C24" s="7"/>
       <c r="D24" s="7"/>
       <c r="E24" s="7"/>
-    </row>
-    <row r="25" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
+      <c r="F24" s="7"/>
+    </row>
+    <row r="25" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="A25" s="5"/>
+      <c r="B25" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="B25" s="7"/>
       <c r="C25" s="7"/>
       <c r="D25" s="7"/>
       <c r="E25" s="7"/>
-    </row>
-    <row r="26" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="F25" s="7"/>
+    </row>
+    <row r="26" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
-      <c r="B26" s="7" t="s">
+      <c r="B26" s="7"/>
+      <c r="C26" s="7" t="s">
         <v>134</v>
       </c>
-      <c r="C26" s="7">
+      <c r="D26" s="7">
         <v>15</v>
       </c>
-      <c r="D26" s="7" t="s">
+      <c r="E26" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="E26" s="7" t="s">
+      <c r="F26" s="7" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
+    <row r="27" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="A27" s="4"/>
+      <c r="B27" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="B27" s="7"/>
       <c r="C27" s="7"/>
       <c r="D27" s="7"/>
       <c r="E27" s="7"/>
-    </row>
-    <row r="28" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
+      <c r="F27" s="7"/>
+    </row>
+    <row r="28" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="A28" s="5"/>
+      <c r="B28" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="B28" s="7"/>
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
       <c r="E28" s="7"/>
-    </row>
-    <row r="29" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="F28" s="7"/>
+    </row>
+    <row r="29" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
-      <c r="B29" s="7" t="s">
+      <c r="B29" s="7"/>
+      <c r="C29" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="C29" s="7">
+      <c r="D29" s="7">
         <v>5</v>
       </c>
-      <c r="D29" s="7" t="s">
+      <c r="E29" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="E29" s="7" t="s">
+      <c r="F29" s="7" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
+    <row r="30" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="A30" s="4"/>
+      <c r="B30" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="B30" s="7"/>
       <c r="C30" s="7"/>
       <c r="D30" s="7"/>
       <c r="E30" s="7"/>
-    </row>
-    <row r="31" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A31" s="5" t="s">
+      <c r="F30" s="7"/>
+    </row>
+    <row r="31" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="A31" s="5"/>
+      <c r="B31" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="B31" s="7"/>
       <c r="C31" s="7"/>
       <c r="D31" s="7"/>
       <c r="E31" s="7"/>
-    </row>
-    <row r="32" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="F31" s="7"/>
+    </row>
+    <row r="32" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
-      <c r="B32" s="7" t="s">
+      <c r="B32" s="7"/>
+      <c r="C32" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="C32" s="7">
+      <c r="D32" s="7">
         <v>5</v>
       </c>
-      <c r="D32" s="7" t="s">
+      <c r="E32" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="E32" s="7" t="s">
+      <c r="F32" s="7" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A33" s="4" t="s">
+    <row r="33" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="A33" s="4"/>
+      <c r="B33" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="B33" s="7"/>
       <c r="C33" s="7"/>
       <c r="D33" s="7"/>
       <c r="E33" s="7"/>
-    </row>
-    <row r="34" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A34" s="5" t="s">
+      <c r="F33" s="7"/>
+    </row>
+    <row r="34" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="A34" s="5"/>
+      <c r="B34" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="B34" s="7"/>
       <c r="C34" s="7"/>
       <c r="D34" s="7"/>
       <c r="E34" s="7"/>
-    </row>
-    <row r="35" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="F34" s="7"/>
+    </row>
+    <row r="35" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A35" s="3"/>
-      <c r="B35" s="7" t="s">
+      <c r="B35" s="7"/>
+      <c r="C35" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="C35" s="7">
+      <c r="D35" s="7">
         <v>54</v>
       </c>
-      <c r="D35" s="7" t="s">
+      <c r="E35" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="E35" s="7" t="s">
+      <c r="F35" s="7" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A36" s="4" t="s">
+    <row r="36" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="A36" s="4"/>
+      <c r="B36" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="B36" s="7"/>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
-    </row>
-    <row r="37" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A37" s="5" t="s">
+      <c r="F36" s="7"/>
+    </row>
+    <row r="37" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="A37" s="5"/>
+      <c r="B37" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="B37" s="7"/>
       <c r="C37" s="7"/>
       <c r="D37" s="7"/>
       <c r="E37" s="7"/>
-    </row>
-    <row r="38" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="F37" s="7"/>
+    </row>
+    <row r="38" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A38" s="3"/>
-      <c r="B38" s="7" t="s">
+      <c r="B38" s="7"/>
+      <c r="C38" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="C38" s="7">
+      <c r="D38" s="7">
         <v>10</v>
       </c>
-      <c r="D38" s="7" t="s">
+      <c r="E38" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="E38" s="7" t="s">
+      <c r="F38" s="7" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A39" s="4" t="s">
+    <row r="39" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="A39" s="4"/>
+      <c r="B39" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="B39" s="7"/>
       <c r="C39" s="7"/>
       <c r="D39" s="7"/>
       <c r="E39" s="7"/>
-    </row>
-    <row r="40" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A40" s="5" t="s">
+      <c r="F39" s="7"/>
+    </row>
+    <row r="40" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="A40" s="5"/>
+      <c r="B40" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="B40" s="7"/>
       <c r="C40" s="7"/>
       <c r="D40" s="7"/>
       <c r="E40" s="7"/>
-    </row>
-    <row r="41" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="F40" s="7"/>
+    </row>
+    <row r="41" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A41" s="3"/>
-      <c r="B41" s="7" t="s">
+      <c r="B41" s="7"/>
+      <c r="C41" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="C41" s="7">
+      <c r="D41" s="7">
         <v>34</v>
       </c>
-      <c r="D41" s="7" t="s">
+      <c r="E41" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="E41" s="7" t="s">
+      <c r="F41" s="7" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A42" s="4" t="s">
+    <row r="42" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="A42" s="4"/>
+      <c r="B42" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="B42" s="7"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
-    </row>
-    <row r="43" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A43" s="5" t="s">
+      <c r="F42" s="7"/>
+    </row>
+    <row r="43" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="A43" s="5"/>
+      <c r="B43" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="B43" s="7"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
-    </row>
-    <row r="44" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="F43" s="7"/>
+    </row>
+    <row r="44" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A44" s="3"/>
-      <c r="B44" s="7" t="s">
+      <c r="B44" s="7"/>
+      <c r="C44" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="C44" s="7">
+      <c r="D44" s="7">
         <v>20</v>
       </c>
-      <c r="D44" s="7" t="s">
+      <c r="E44" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="E44" s="7" t="s">
+      <c r="F44" s="7" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A45" s="4" t="s">
+    <row r="45" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="A45" s="4"/>
+      <c r="B45" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="B45" s="7"/>
       <c r="C45" s="7"/>
       <c r="D45" s="7"/>
       <c r="E45" s="7"/>
-    </row>
-    <row r="46" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A46" s="5" t="s">
+      <c r="F45" s="7"/>
+    </row>
+    <row r="46" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="A46" s="5"/>
+      <c r="B46" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="B46" s="7"/>
       <c r="C46" s="7"/>
       <c r="D46" s="7"/>
       <c r="E46" s="7"/>
-    </row>
-    <row r="47" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="F46" s="7"/>
+    </row>
+    <row r="47" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A47" s="3"/>
-      <c r="B47" s="7" t="s">
+      <c r="B47" s="7"/>
+      <c r="C47" s="7" t="s">
         <v>162</v>
       </c>
-      <c r="C47" s="7">
+      <c r="D47" s="7">
         <v>60</v>
       </c>
-      <c r="D47" s="7" t="s">
+      <c r="E47" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="E47" s="7" t="s">
+      <c r="F47" s="7" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A48" s="4" t="s">
+    <row r="48" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="A48" s="4"/>
+      <c r="B48" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="B48" s="7"/>
       <c r="C48" s="7"/>
       <c r="D48" s="7"/>
       <c r="E48" s="7"/>
-    </row>
-    <row r="49" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A49" s="5" t="s">
+      <c r="F48" s="7"/>
+    </row>
+    <row r="49" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="A49" s="5"/>
+      <c r="B49" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="B49" s="7"/>
       <c r="C49" s="7"/>
       <c r="D49" s="7"/>
       <c r="E49" s="7"/>
-    </row>
-    <row r="50" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="F49" s="7"/>
+    </row>
+    <row r="50" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A50" s="3"/>
-      <c r="B50" s="7" t="s">
+      <c r="B50" s="7"/>
+      <c r="C50" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="C50" s="7">
+      <c r="D50" s="7">
         <v>20</v>
       </c>
-      <c r="D50" s="7" t="s">
+      <c r="E50" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="E50" s="7" t="s">
+      <c r="F50" s="7" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A51" s="4" t="s">
+    <row r="51" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="A51" s="4"/>
+      <c r="B51" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="B51" s="7"/>
       <c r="C51" s="7"/>
       <c r="D51" s="7"/>
       <c r="E51" s="7"/>
-    </row>
-    <row r="52" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A52" s="5" t="s">
+      <c r="F51" s="7"/>
+    </row>
+    <row r="52" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="A52" s="5"/>
+      <c r="B52" s="5" t="s">
         <v>165</v>
       </c>
-      <c r="B52" s="7"/>
       <c r="C52" s="7"/>
       <c r="D52" s="7"/>
       <c r="E52" s="7"/>
-    </row>
-    <row r="53" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="F52" s="7"/>
+    </row>
+    <row r="53" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A53" s="3"/>
-      <c r="B53" s="7" t="s">
+      <c r="B53" s="7"/>
+      <c r="C53" s="7" t="s">
         <v>170</v>
       </c>
-      <c r="C53" s="7">
+      <c r="D53" s="7">
         <v>20</v>
       </c>
-      <c r="D53" s="7" t="s">
+      <c r="E53" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="E53" s="7" t="s">
+      <c r="F53" s="7" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A54" s="4" t="s">
+    <row r="54" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="A54" s="4"/>
+      <c r="B54" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="B54" s="7"/>
       <c r="C54" s="7"/>
       <c r="D54" s="7"/>
       <c r="E54" s="7"/>
-    </row>
-    <row r="55" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A55" s="5" t="s">
+      <c r="F54" s="7"/>
+    </row>
+    <row r="55" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="A55" s="5"/>
+      <c r="B55" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="B55" s="7"/>
       <c r="C55" s="7"/>
       <c r="D55" s="7"/>
       <c r="E55" s="7"/>
-    </row>
-    <row r="56" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="F55" s="7"/>
+    </row>
+    <row r="56" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A56" s="3"/>
-      <c r="B56" s="7" t="s">
+      <c r="B56" s="7"/>
+      <c r="C56" s="7" t="s">
         <v>173</v>
       </c>
-      <c r="C56" s="7">
+      <c r="D56" s="7">
         <v>20</v>
       </c>
-      <c r="D56" s="7" t="s">
+      <c r="E56" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="E56" s="7" t="s">
+      <c r="F56" s="7" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="57" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A57" s="4" t="s">
+    <row r="57" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="A57" s="4"/>
+      <c r="B57" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="B57" s="7"/>
       <c r="C57" s="7"/>
       <c r="D57" s="7"/>
       <c r="E57" s="7"/>
-    </row>
-    <row r="58" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A58" s="5" t="s">
+      <c r="F57" s="7"/>
+    </row>
+    <row r="58" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="A58" s="5"/>
+      <c r="B58" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="B58" s="7"/>
       <c r="C58" s="7"/>
       <c r="D58" s="7"/>
       <c r="E58" s="7"/>
-    </row>
-    <row r="59" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="F58" s="7"/>
+    </row>
+    <row r="59" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A59" s="3"/>
-      <c r="B59" s="7" t="s">
+      <c r="B59" s="7"/>
+      <c r="C59" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="C59" s="7">
+      <c r="D59" s="7">
         <v>35</v>
       </c>
-      <c r="D59" s="7" t="s">
+      <c r="E59" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="E59" s="7" t="s">
+      <c r="F59" s="7" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A60" s="4" t="s">
+    <row r="60" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="A60" s="4"/>
+      <c r="B60" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="B60" s="7"/>
       <c r="C60" s="7"/>
       <c r="D60" s="7"/>
       <c r="E60" s="7"/>
-    </row>
-    <row r="61" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A61" s="5" t="s">
+      <c r="F60" s="7"/>
+    </row>
+    <row r="61" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="A61" s="5"/>
+      <c r="B61" s="5" t="s">
         <v>176</v>
       </c>
-      <c r="B61" s="7"/>
       <c r="C61" s="7"/>
       <c r="D61" s="7"/>
       <c r="E61" s="7"/>
-    </row>
-    <row r="62" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="F61" s="7"/>
+    </row>
+    <row r="62" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A62" s="3"/>
-      <c r="B62" s="7" t="s">
+      <c r="B62" s="7"/>
+      <c r="C62" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="C62" s="7">
+      <c r="D62" s="7">
         <v>5</v>
       </c>
-      <c r="D62" s="7" t="s">
+      <c r="E62" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="E62" s="7" t="s">
+      <c r="F62" s="7" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A63" s="4" t="s">
+    <row r="63" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="A63" s="4"/>
+      <c r="B63" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="B63" s="7"/>
       <c r="C63" s="7"/>
       <c r="D63" s="7"/>
       <c r="E63" s="7"/>
-    </row>
-    <row r="64" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A64" s="5" t="s">
+      <c r="F63" s="7"/>
+    </row>
+    <row r="64" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="A64" s="5"/>
+      <c r="B64" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="B64" s="7"/>
       <c r="C64" s="7"/>
       <c r="D64" s="7"/>
       <c r="E64" s="7"/>
-    </row>
-    <row r="65" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="F64" s="7"/>
+    </row>
+    <row r="65" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A65" s="3"/>
-      <c r="B65" s="7" t="s">
+      <c r="B65" s="7"/>
+      <c r="C65" s="7" t="s">
         <v>185</v>
       </c>
-      <c r="C65" s="7">
+      <c r="D65" s="7">
         <v>10</v>
       </c>
-      <c r="D65" s="7" t="s">
+      <c r="E65" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="E65" s="7" t="s">
+      <c r="F65" s="7" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="66" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A66" s="4" t="s">
+    <row r="66" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="A66" s="4"/>
+      <c r="B66" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="B66" s="7"/>
       <c r="C66" s="7"/>
       <c r="D66" s="7"/>
       <c r="E66" s="7"/>
-    </row>
-    <row r="67" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A67" s="5" t="s">
+      <c r="F66" s="7"/>
+    </row>
+    <row r="67" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="A67" s="5"/>
+      <c r="B67" s="5" t="s">
         <v>184</v>
       </c>
-      <c r="B67" s="7"/>
       <c r="C67" s="7"/>
       <c r="D67" s="7"/>
       <c r="E67" s="7"/>
-    </row>
-    <row r="68" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="F67" s="7"/>
+    </row>
+    <row r="68" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A68" s="3"/>
-      <c r="B68" s="7" t="s">
+      <c r="B68" s="7"/>
+      <c r="C68" s="7" t="s">
         <v>189</v>
       </c>
-      <c r="C68" s="7">
+      <c r="D68" s="7">
         <v>35</v>
       </c>
-      <c r="D68" s="7" t="s">
+      <c r="E68" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="E68" s="7" t="s">
+      <c r="F68" s="7" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="69" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A69" s="4" t="s">
+    <row r="69" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="A69" s="4"/>
+      <c r="B69" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="B69" s="7"/>
       <c r="C69" s="7"/>
       <c r="D69" s="7"/>
       <c r="E69" s="7"/>
-    </row>
-    <row r="70" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A70" s="5" t="s">
+      <c r="F69" s="7"/>
+    </row>
+    <row r="70" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="A70" s="5"/>
+      <c r="B70" s="5" t="s">
         <v>188</v>
       </c>
-      <c r="B70" s="7"/>
       <c r="C70" s="7"/>
       <c r="D70" s="7"/>
       <c r="E70" s="7"/>
-    </row>
-    <row r="71" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="F70" s="7"/>
+    </row>
+    <row r="71" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A71" s="3"/>
-      <c r="B71" s="7" t="s">
+      <c r="B71" s="7"/>
+      <c r="C71" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="C71" s="7">
+      <c r="D71" s="7">
         <v>5</v>
       </c>
-      <c r="D71" s="7" t="s">
+      <c r="E71" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="E71" s="7" t="s">
+      <c r="F71" s="7" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="72" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A72" s="4" t="s">
+    <row r="72" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="A72" s="4"/>
+      <c r="B72" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="B72" s="7"/>
       <c r="C72" s="7"/>
       <c r="D72" s="7"/>
       <c r="E72" s="7"/>
-    </row>
-    <row r="73" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A73" s="5" t="s">
+      <c r="F72" s="7"/>
+    </row>
+    <row r="73" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="A73" s="5"/>
+      <c r="B73" s="5" t="s">
         <v>192</v>
       </c>
-      <c r="B73" s="7"/>
       <c r="C73" s="7"/>
       <c r="D73" s="7"/>
       <c r="E73" s="7"/>
-    </row>
-    <row r="74" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="F73" s="7"/>
+    </row>
+    <row r="74" spans="1:6" ht="19" x14ac:dyDescent="0.25">
       <c r="A74" s="3"/>
-      <c r="B74" s="7" t="s">
+      <c r="B74" s="7"/>
+      <c r="C74" s="7" t="s">
         <v>197</v>
       </c>
-      <c r="C74" s="7">
+      <c r="D74" s="7">
         <v>20</v>
       </c>
-      <c r="D74" s="7" t="s">
+      <c r="E74" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="E74" s="7" t="s">
+      <c r="F74" s="7" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="75" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A75" s="4" t="s">
+    <row r="75" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="A75" s="4"/>
+      <c r="B75" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="B75" s="7"/>
       <c r="C75" s="7"/>
       <c r="D75" s="7"/>
       <c r="E75" s="7"/>
-    </row>
-    <row r="76" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A76" s="5" t="s">
+      <c r="F75" s="7"/>
+    </row>
+    <row r="76" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="A76" s="5"/>
+      <c r="B76" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="B76" s="7"/>
       <c r="C76" s="7"/>
       <c r="D76" s="7"/>
       <c r="E76" s="7"/>
-    </row>
-    <row r="77" spans="1:5" ht="19" x14ac:dyDescent="0.25">
-      <c r="A77" s="6" t="s">
+      <c r="F76" s="7"/>
+    </row>
+    <row r="77" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+      <c r="A77" s="6"/>
+      <c r="B77" s="6" t="s">
         <v>199</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="96">
-    <mergeCell ref="B71:B73"/>
-    <mergeCell ref="C71:C73"/>
-    <mergeCell ref="D71:D73"/>
-    <mergeCell ref="E71:E73"/>
-    <mergeCell ref="B74:B76"/>
-    <mergeCell ref="C74:C76"/>
-    <mergeCell ref="D74:D76"/>
-    <mergeCell ref="E74:E76"/>
-    <mergeCell ref="B65:B67"/>
-    <mergeCell ref="C65:C67"/>
-    <mergeCell ref="D65:D67"/>
-    <mergeCell ref="E65:E67"/>
-    <mergeCell ref="B68:B70"/>
-    <mergeCell ref="C68:C70"/>
-    <mergeCell ref="D68:D70"/>
-    <mergeCell ref="E68:E70"/>
-    <mergeCell ref="B59:B61"/>
-    <mergeCell ref="C59:C61"/>
-    <mergeCell ref="D59:D61"/>
-    <mergeCell ref="E59:E61"/>
-    <mergeCell ref="B62:B64"/>
-    <mergeCell ref="C62:C64"/>
-    <mergeCell ref="D62:D64"/>
-    <mergeCell ref="E62:E64"/>
-    <mergeCell ref="B53:B55"/>
-    <mergeCell ref="C53:C55"/>
-    <mergeCell ref="D53:D55"/>
-    <mergeCell ref="E53:E55"/>
-    <mergeCell ref="B56:B58"/>
-    <mergeCell ref="C56:C58"/>
-    <mergeCell ref="D56:D58"/>
-    <mergeCell ref="E56:E58"/>
-    <mergeCell ref="B47:B49"/>
-    <mergeCell ref="C47:C49"/>
-    <mergeCell ref="D47:D49"/>
-    <mergeCell ref="E47:E49"/>
-    <mergeCell ref="B50:B52"/>
-    <mergeCell ref="C50:C52"/>
-    <mergeCell ref="D50:D52"/>
-    <mergeCell ref="E50:E52"/>
-    <mergeCell ref="B41:B43"/>
-    <mergeCell ref="C41:C43"/>
-    <mergeCell ref="D41:D43"/>
-    <mergeCell ref="E41:E43"/>
-    <mergeCell ref="B44:B46"/>
-    <mergeCell ref="C44:C46"/>
-    <mergeCell ref="D44:D46"/>
-    <mergeCell ref="E44:E46"/>
-    <mergeCell ref="B35:B37"/>
-    <mergeCell ref="C35:C37"/>
-    <mergeCell ref="D35:D37"/>
-    <mergeCell ref="E35:E37"/>
-    <mergeCell ref="B38:B40"/>
-    <mergeCell ref="C38:C40"/>
-    <mergeCell ref="D38:D40"/>
-    <mergeCell ref="E38:E40"/>
-    <mergeCell ref="B29:B31"/>
-    <mergeCell ref="C29:C31"/>
-    <mergeCell ref="D29:D31"/>
-    <mergeCell ref="E29:E31"/>
-    <mergeCell ref="B32:B34"/>
-    <mergeCell ref="C32:C34"/>
-    <mergeCell ref="D32:D34"/>
-    <mergeCell ref="E32:E34"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="C23:C25"/>
-    <mergeCell ref="D23:D25"/>
-    <mergeCell ref="E23:E25"/>
-    <mergeCell ref="B26:B28"/>
-    <mergeCell ref="C26:C28"/>
-    <mergeCell ref="D26:D28"/>
-    <mergeCell ref="E26:E28"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="C17:C19"/>
-    <mergeCell ref="D17:D19"/>
-    <mergeCell ref="E17:E19"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="D20:D22"/>
-    <mergeCell ref="E20:E22"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="D11:D13"/>
-    <mergeCell ref="E11:E13"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="C14:C16"/>
-    <mergeCell ref="D14:D16"/>
-    <mergeCell ref="E14:E16"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="E5:E7"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="E8:E10"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>